<commit_message>
conversion to sample tab from excel
</commit_message>
<xml_diff>
--- a/t/data/Excel/faang_metadata_examples_macleod_horses_20160205.xlsx
+++ b/t/data/Excel/faang_metadata_examples_macleod_horses_20160205.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6100" yWindow="2280" windowWidth="25600" windowHeight="16060" tabRatio="612" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="6100" yWindow="2280" windowWidth="25600" windowHeight="16060" tabRatio="612" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="6" r:id="rId1"/>
@@ -1271,7 +1271,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="291">
+  <cellStyleXfs count="292">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1550,6 +1550,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1602,7 +1603,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="291">
+  <cellStyles count="292">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1788,6 +1789,7 @@
     <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="289" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="291" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3365,7 +3367,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -3398,16 +3402,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" s="6" t="s">
         <v>317</v>
       </c>
@@ -3421,25 +3429,25 @@
         <v>320</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>321</v>
       </c>
       <c r="B2" t="s">
         <v>322</v>
       </c>
+      <c r="C2" t="s">
+        <v>323</v>
+      </c>
       <c r="D2" t="s">
-        <v>323</v>
-      </c>
-      <c r="E2" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17">
+    <row r="3" spans="1:4" ht="17">
       <c r="B3" s="31"/>
       <c r="C3" s="31"/>
     </row>
-    <row r="4" spans="1:5" ht="17">
+    <row r="4" spans="1:4" ht="17">
       <c r="B4" s="31"/>
       <c r="C4" s="31"/>
     </row>
@@ -3514,11 +3522,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">

</xml_diff>